<commit_message>
revise the sentence number in MuST-C
</commit_message>
<xml_diff>
--- a/speech_translation_corpus.xlsx
+++ b/speech_translation_corpus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyuchen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyuchen/Documents/GitHub/speech_translation-papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4575F733-80A5-E242-A573-4A3370582BA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B0A895-BB04-4942-ACF8-9B295627A7A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="960" windowWidth="24540" windowHeight="14020" xr2:uid="{849F8198-8890-394B-9801-24C70A052DAE}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14500" xr2:uid="{849F8198-8890-394B-9801-24C70A052DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,10 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.0M~5.3M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>190K~345K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -398,6 +394,10 @@
   </si>
   <si>
     <t>注：1-5论文中较常见，6-8今年新提出的数据集，9视频音频字幕翻译多模态数据，10低资源小语种，11同传数据集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>211K~280K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -655,34 +655,34 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6C0615-9D1C-5843-9227-E281DBEBD7D1}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1016,41 +1016,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1073,10 +1073,10 @@
         <v>171121</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1099,10 +1099,10 @@
         <v>131395</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1119,16 +1119,16 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="4">
         <v>153899</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1148,13 +1148,13 @@
         <v>27</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1162,29 +1162,29 @@
         <v>5</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>61</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="32">
+      <c r="A8" s="30">
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1200,17 +1200,17 @@
         <v>4</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="32">
+      <c r="A9" s="30">
         <v>7</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -1236,7 +1236,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="32">
+      <c r="A10" s="30">
         <v>8</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -1249,10 +1249,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>22</v>
@@ -1262,33 +1262,33 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="32">
+      <c r="A11" s="30">
         <v>9</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>47</v>
       </c>
       <c r="F11" s="16">
         <v>184949</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="32">
+      <c r="A12" s="30">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1304,58 +1304,58 @@
         <v>2</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="32">
+      <c r="A13" s="30">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="A15" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>